<commit_message>
graphe ia design actuel
</commit_message>
<xml_diff>
--- a/DM3/ia.xlsx
+++ b/DM3/ia.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\ift3911\DM2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\ift3911\DM3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>I</t>
   </si>
@@ -48,33 +48,6 @@
     <t>paquet</t>
   </si>
   <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>trip</t>
-  </si>
-  <si>
-    <t>reservation</t>
-  </si>
-  <si>
-    <t>payment</t>
-  </si>
-  <si>
-    <t>usersessions</t>
-  </si>
-  <si>
-    <t>utils</t>
-  </si>
-  <si>
-    <t>livestorage</t>
-  </si>
-  <si>
-    <t>persistantstorage</t>
-  </si>
-  <si>
-    <t>gui</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -85,6 +58,60 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Sessions</t>
+  </si>
+  <si>
+    <t>Utils</t>
+  </si>
+  <si>
+    <t>Commands</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Réservation</t>
+  </si>
+  <si>
+    <t>Paiment</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Travel.Facilities</t>
+  </si>
+  <si>
+    <t>Travel.Trip</t>
+  </si>
+  <si>
+    <t>Travel.Vehicule</t>
+  </si>
+  <si>
+    <t>Travel.Factories</t>
+  </si>
+  <si>
+    <t>Travel.Forms</t>
+  </si>
+  <si>
+    <t>Travel.Itineries</t>
+  </si>
+  <si>
+    <t>Travel.Sections</t>
+  </si>
+  <si>
+    <t>Travel.Places</t>
+  </si>
+  <si>
+    <t>Travel.</t>
+  </si>
+  <si>
+    <t>Travel.VechiculeModels</t>
   </si>
 </sst>
 </file>
@@ -258,30 +285,57 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.66666666666666663</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.75</c:v>
+                  <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.66666666666666663</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -294,31 +348,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21568627450980393</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.23076923076923078</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.33333333333333331</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.33333333333333331</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.66666666666666663</c:v>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -591,11 +672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136096848"/>
-        <c:axId val="136097632"/>
+        <c:axId val="443652632"/>
+        <c:axId val="443653808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136096848"/>
+        <c:axId val="443652632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -705,12 +786,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136097632"/>
+        <c:crossAx val="443653808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136097632"/>
+        <c:axId val="443653808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -819,7 +900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136096848"/>
+        <c:crossAx val="443652632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1423,7 +1504,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1723,13 +1804,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -1757,227 +1838,227 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <f>D2/(E2+D2)</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C2">
-        <f>F2/G2</f>
-        <v>0.25</v>
+        <f>F2/(G2+F2)</f>
+        <v>0</v>
       </c>
       <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3" si="0">D3/(E3+D3)</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3" si="1">F3/G3</f>
-        <v>0.23076923076923078</v>
+        <f t="shared" ref="C3:C9" si="1">F3/(G3+F3)</f>
+        <v>0.36363636363636365</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B10" si="2">D4/(E4+D4)</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C10" si="3">F4/G4</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <f t="shared" si="2"/>
-        <v>0.83333333333333337</v>
+        <v>0.9375</v>
       </c>
       <c r="C5">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="C6">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
+        <f t="shared" si="1"/>
+        <v>0.21568627450980393</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="B9" si="3">D9/(E9+D9)</f>
+        <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
       <c r="V9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="W9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="X9" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="Y9" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
+        <f>D10/(E10+D10)</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="C10:C19" si="4">F10/(G10+F10)</f>
+        <v>0.25</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1986,7 +2067,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -2003,6 +2084,29 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B10:B19" si="5">D11/(E11+D11)</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
       <c r="V11">
         <v>1</v>
       </c>
@@ -2013,7 +2117,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V13">
         <v>0</v>
       </c>
@@ -2022,6 +2150,17 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V14">
         <v>0.5</v>
       </c>
@@ -2029,7 +2168,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C16" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V16">
         <v>0.5</v>
       </c>
@@ -2037,7 +2200,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V17">
         <v>1</v>
       </c>
@@ -2045,7 +2219,31 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C18" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="V19">
         <v>0</v>
       </c>
@@ -2053,7 +2251,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V20">
         <v>0.75</v>
       </c>
@@ -2061,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V22">
         <v>0.25</v>
       </c>
@@ -2069,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="22:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V23">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
discussion sur la qualité bien entamée, graphe IA.
</commit_message>
<xml_diff>
--- a/DM3/ia.xlsx
+++ b/DM3/ia.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$G$19</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>I</t>
   </si>
@@ -91,6 +94,9 @@
   </si>
   <si>
     <t>Travel.Vehicule</t>
+  </si>
+  <si>
+    <t>Travel.Factories</t>
   </si>
   <si>
     <t>Travel.Forms</t>
@@ -282,7 +288,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
@@ -291,13 +297,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9375</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>9.0909090909090912E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -309,28 +315,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.55555555555555558</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.65116279069767447</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -342,43 +351,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.21568627450980393</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.21428571428571427</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.125</c:v>
+                  <c:v>0.19047619047619047</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0.15384615384615385</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -390,6 +399,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1495,7 +1507,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1795,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,27 +1841,27 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <f>D2/(E2+D2)</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>F2/(G2+F2)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1857,11 +1869,11 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3" si="0">D3/(E3+D3)</f>
+        <f>D3/(E3+D3)</f>
         <v>0.5</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="1">F3/(G3+F3)</f>
+        <f>F3/(G3+F3)</f>
         <v>0.36363636363636365</v>
       </c>
       <c r="D3">
@@ -1879,52 +1891,52 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B10" si="2">D4/(E4+D4)</f>
+        <f>D4/(E4+D4)</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f>F4/(G4+F4)</f>
+        <v>0.25</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <f t="shared" si="2"/>
-        <v>0.9375</v>
+        <f>D5/(E5+D5)</f>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F5/(G5+F5)</f>
+        <v>0.25</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -1932,11 +1944,11 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <f t="shared" si="2"/>
+        <f>D6/(E6+D6)</f>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f>F6/(G6+F6)</f>
         <v>0.21568627450980393</v>
       </c>
       <c r="D6">
@@ -1954,40 +1966,40 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
+        <f>D7/(E7+D7)</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <f>F7/(G7+F7)</f>
+        <v>0.21428571428571427</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <f t="shared" si="2"/>
+        <f>D8/(E8+D8)</f>
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>F8/(G8+F8)</f>
+        <v>0.2</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1999,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -2007,11 +2019,11 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9" si="3">D9/(E9+D9)</f>
+        <f>D9/(E9+D9)</f>
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f>F9/(G9+F9)</f>
         <v>0.2</v>
       </c>
       <c r="D9">
@@ -2041,27 +2053,27 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <f>D10/(E10+D10)</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:C19" si="4">F10/(G10+F10)</f>
-        <v>0.25</v>
+        <f>F10/(G10+F10)</f>
+        <v>0.2</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -2076,27 +2088,27 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B10:B19" si="5">D11/(E11+D11)</f>
-        <v>0.66666666666666663</v>
+        <f>D11/(E11+D11)</f>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="4"/>
-        <v>0.125</v>
+        <f>F11/(G11+F11)</f>
+        <v>0.19047619047619047</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="V11">
         <v>1</v>
@@ -2110,15 +2122,15 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <f t="shared" si="5"/>
+        <f>D12/(E12+D12)</f>
         <v>0.5</v>
       </c>
       <c r="C12">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
+        <f>F12/(G12+F12)</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2130,32 +2142,32 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:B18" si="6">D13/(E13+D13)</f>
-        <v>0.55555555555555558</v>
+        <f>D13/(E13+D13)</f>
+        <v>0.77777777777777779</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C18" si="7">F13/(G13+F13)</f>
-        <v>0</v>
+        <f>F13/(G13+F13)</f>
+        <v>0.15384615384615385</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2166,27 +2178,27 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>D14/(E14+D14)</f>
+        <v>0.75</v>
       </c>
       <c r="C14">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
+        <f>F14/(G14+F14)</f>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <v>0.5</v>
@@ -2197,28 +2209,52 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C15" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>D15/(E15+D15)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="C15">
+        <f>F15/(G15+F15)</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <f>D16/(E16+D16)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C16">
+        <f>F16/(G16+F16)</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
       </c>
       <c r="V16">
         <v>0.5</v>
@@ -2231,13 +2267,25 @@
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="B17">
+        <f>D17/(E17+D17)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C17">
+        <f>F17/(G17+F17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
       </c>
       <c r="V17">
         <v>1</v>
@@ -2250,16 +2298,51 @@
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="B18">
+        <f>D18/(E18+D18)</f>
+        <v>0.8</v>
+      </c>
+      <c r="C18">
+        <f>F18/(G18+F18)</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <f>D19/(E19+D19)</f>
+        <v>0.65116279069767447</v>
+      </c>
+      <c r="C19">
+        <f>F19/(G19+F19)</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
       <c r="V19">
         <v>0</v>
       </c>
@@ -2292,6 +2375,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G19">
+    <sortState ref="A2:G19">
+      <sortCondition descending="1" ref="C1:C19"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Frame par interface graphique
</commit_message>
<xml_diff>
--- a/DM3/ia.xlsx
+++ b/DM3/ia.xlsx
@@ -396,7 +396,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1808,7 +1808,7 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="C17">
         <f>F17/(G17+F17)</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2282,10 +2282,10 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V17">
         <v>1</v>

</xml_diff>